<commit_message>
Add Yaouw Volcano and Dune Hot's Peak
</commit_message>
<xml_diff>
--- a/data/Data Spreadsheet.xlsx
+++ b/data/Data Spreadsheet.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Dropbox\Projects\Toshe's Underwater Adventures\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621"/>
+    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EXP" sheetId="2" r:id="rId1"/>
@@ -26,12 +21,12 @@
     <sheet name="Coliseum" sheetId="14" r:id="rId12"/>
     <sheet name="Coliseum Text" sheetId="16" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3224" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3242" uniqueCount="1286">
   <si>
     <t>Club</t>
   </si>
@@ -3862,6 +3857,33 @@
   </si>
   <si>
     <t>{'Hot Coals': 20, 'Melting Touch': 15, 'Scorch': 40, 'Healing Ray': 15, 'Firestorm': 10}</t>
+  </si>
+  <si>
+    <t>Animated Magma</t>
+  </si>
+  <si>
+    <t>Tectonic Beast</t>
+  </si>
+  <si>
+    <t>{'Molten Rocks': 5, 'Hot Coals': 15, 'Scorch': 10, 'Immolation': 20, 'Strong Attack': 50}</t>
+  </si>
+  <si>
+    <t>{'Rock Shield': 10, 'Glowing Barrier': 5}</t>
+  </si>
+  <si>
+    <t>{'Fireball': 30, 'Avalanche': 14, 'Fumarole': 6, 'Strong Attack': 30, 'Immolation': 20}</t>
+  </si>
+  <si>
+    <t>{'Rock Shield': 5, 'Flame Guard': 35, 'Flametongue': 60}</t>
+  </si>
+  <si>
+    <t>Duner</t>
+  </si>
+  <si>
+    <t>{'Quicksand': 4, 'Duststorm': 2, 'Battery Cage': 6}</t>
+  </si>
+  <si>
+    <t>Game Over Theme</t>
   </si>
 </sst>
 </file>
@@ -4676,7 +4698,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5047,12 +5068,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126971056"/>
-        <c:axId val="126005824"/>
+        <c:axId val="89037440"/>
+        <c:axId val="89039232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126971056"/>
+        <c:axId val="89037440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5062,7 +5084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126005824"/>
+        <c:crossAx val="89039232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5070,7 +5092,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126005824"/>
+        <c:axId val="89039232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000"/>
@@ -5082,14 +5104,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126971056"/>
+        <c:crossAx val="89037440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5119,7 +5140,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5773,12 +5793,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="124895992"/>
-        <c:axId val="124896384"/>
+        <c:axId val="105145088"/>
+        <c:axId val="105147008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124895992"/>
+        <c:axId val="105145088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5800,14 +5821,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124896384"/>
+        <c:crossAx val="105147008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5817,7 +5837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124896384"/>
+        <c:axId val="105147008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5828,14 +5848,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124895992"/>
+        <c:crossAx val="105145088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5963,7 +5982,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5998,7 +6017,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6212,7 +6231,7 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -12682,7 +12701,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:F51"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13725,8 +13744,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14938,13 +14957,13 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Y225"/>
+  <dimension ref="A1:Y228"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="R200" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:Y225"/>
+      <selection pane="bottomRight" activeCell="W228" sqref="W228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31842,31 +31861,31 @@
     </row>
     <row r="220" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A220" s="13" t="s">
-        <v>1182</v>
+        <v>1277</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>1182</v>
+        <v>1277</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>1182</v>
+        <v>1277</v>
       </c>
       <c r="D220" s="23">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E220" s="33">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="F220" s="35">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="G220" s="41">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H220" s="25">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I220" s="24">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="J220" s="34">
         <v>200</v>
@@ -31875,28 +31894,28 @@
         <v>0</v>
       </c>
       <c r="L220" s="27">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="M220" s="17">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N220" s="3">
-        <v>-50</v>
+        <v>-100</v>
       </c>
       <c r="O220" s="29">
         <v>100</v>
       </c>
       <c r="P220" s="18">
-        <v>25</v>
-      </c>
-      <c r="Q220" s="2" t="s">
-        <v>1225</v>
+        <v>50</v>
+      </c>
+      <c r="Q220" t="s">
+        <v>1279</v>
       </c>
       <c r="R220" t="s">
-        <v>1206</v>
+        <v>1280</v>
       </c>
       <c r="S220" s="20">
-        <v>3000</v>
+        <v>1700</v>
       </c>
       <c r="T220" s="31">
         <v>0</v>
@@ -31908,39 +31927,39 @@
         <v>0</v>
       </c>
       <c r="W220" s="47" t="s">
-        <v>666</v>
+        <v>155</v>
       </c>
       <c r="X220" s="57">
         <v>0</v>
       </c>
       <c r="Y220" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A221" s="13" t="s">
-        <v>1274</v>
+        <v>1182</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>1274</v>
+        <v>1182</v>
       </c>
       <c r="C221" s="13" t="s">
-        <v>1274</v>
+        <v>1182</v>
       </c>
       <c r="D221" s="23">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E221" s="33">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="F221" s="35">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="G221" s="41">
         <v>25</v>
       </c>
       <c r="H221" s="25">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I221" s="24">
         <v>0.1</v>
@@ -31955,28 +31974,28 @@
         <v>300</v>
       </c>
       <c r="M221" s="17">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="N221" s="3">
-        <v>-17</v>
+        <v>-50</v>
       </c>
       <c r="O221" s="29">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="P221" s="18">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q221" s="2" t="s">
-        <v>1276</v>
+        <v>1225</v>
       </c>
       <c r="R221" t="s">
-        <v>1275</v>
+        <v>1206</v>
       </c>
       <c r="S221" s="20">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="T221" s="31">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="U221" s="38">
         <v>1</v>
@@ -31991,33 +32010,33 @@
         <v>0</v>
       </c>
       <c r="Y221" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A222" s="13" t="s">
-        <v>1183</v>
+        <v>1274</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>1183</v>
+        <v>1274</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>1183</v>
+        <v>1274</v>
       </c>
       <c r="D222" s="23">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E222" s="33">
-        <v>70000</v>
+        <v>30000</v>
       </c>
       <c r="F222" s="35">
-        <v>70000</v>
+        <v>30000</v>
       </c>
       <c r="G222" s="41">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H222" s="25">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="I222" s="24">
         <v>0.1</v>
@@ -32029,31 +32048,31 @@
         <v>0</v>
       </c>
       <c r="L222" s="27">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="M222" s="17">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="N222" s="3">
-        <v>-25</v>
+        <v>-17</v>
       </c>
       <c r="O222" s="29">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="P222" s="18">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q222" s="2" t="s">
-        <v>1224</v>
+        <v>1276</v>
       </c>
       <c r="R222" t="s">
-        <v>1207</v>
+        <v>1275</v>
       </c>
       <c r="S222" s="20">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="T222" s="31">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="U222" s="38">
         <v>1</v>
@@ -32068,36 +32087,36 @@
         <v>0</v>
       </c>
       <c r="Y222" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A223" s="13" t="s">
-        <v>1203</v>
+        <v>1183</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>1203</v>
+        <v>1183</v>
       </c>
       <c r="C223" s="13" t="s">
-        <v>1203</v>
+        <v>1183</v>
       </c>
       <c r="D223" s="23">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E223" s="33">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="F223" s="35">
-        <v>200000</v>
+        <v>70000</v>
       </c>
       <c r="G223" s="41">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="H223" s="25">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I223" s="24">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="J223" s="34">
         <v>200</v>
@@ -32106,69 +32125,69 @@
         <v>0</v>
       </c>
       <c r="L223" s="27">
-        <v>2000</v>
+        <v>450</v>
       </c>
       <c r="M223" s="17">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="N223" s="3">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="O223" s="29">
+        <v>200</v>
+      </c>
+      <c r="P223" s="18">
         <v>50</v>
       </c>
-      <c r="P223" s="18">
-        <v>0</v>
-      </c>
       <c r="Q223" s="2" t="s">
-        <v>1232</v>
+        <v>1224</v>
       </c>
       <c r="R223" t="s">
-        <v>1253</v>
+        <v>1207</v>
       </c>
       <c r="S223" s="20">
-        <v>100000</v>
+        <v>5000</v>
       </c>
       <c r="T223" s="31">
         <v>0</v>
       </c>
       <c r="U223" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V223" s="36">
         <v>0</v>
       </c>
       <c r="W223" s="47" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="X223" s="57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y223" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A224" s="13" t="s">
-        <v>1204</v>
+        <v>1278</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>1204</v>
+        <v>1278</v>
       </c>
       <c r="C224" s="13" t="s">
-        <v>1204</v>
+        <v>1278</v>
       </c>
       <c r="D224" s="23">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E224" s="33">
-        <v>400000</v>
+        <v>50000</v>
       </c>
       <c r="F224" s="35">
-        <v>400000</v>
+        <v>50000</v>
       </c>
       <c r="G224" s="41">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="H224" s="25">
         <v>90</v>
@@ -32183,40 +32202,40 @@
         <v>0</v>
       </c>
       <c r="L224" s="27">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="M224" s="17">
         <v>50</v>
       </c>
       <c r="N224" s="3">
+        <v>-50</v>
+      </c>
+      <c r="O224" s="29">
         <v>100</v>
       </c>
-      <c r="O224" s="29">
-        <v>0</v>
-      </c>
       <c r="P224" s="18">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="Q224" s="2" t="s">
-        <v>1273</v>
-      </c>
-      <c r="R224" t="s">
-        <v>1254</v>
+        <v>1281</v>
+      </c>
+      <c r="R224" s="2" t="s">
+        <v>1282</v>
       </c>
       <c r="S224" s="20">
-        <v>200000</v>
+        <v>9000</v>
       </c>
       <c r="T224" s="31">
         <v>0</v>
       </c>
       <c r="U224" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V224" s="36">
         <v>0</v>
       </c>
       <c r="W224" s="47" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="X224" s="57">
         <v>1</v>
@@ -32227,25 +32246,25 @@
     </row>
     <row r="225" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A225" s="13" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="C225" s="13" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="D225" s="23">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E225" s="33">
-        <v>800000</v>
+        <v>200000</v>
       </c>
       <c r="F225" s="35">
-        <v>800000</v>
+        <v>200000</v>
       </c>
       <c r="G225" s="41">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H225" s="25">
         <v>90</v>
@@ -32266,22 +32285,22 @@
         <v>100</v>
       </c>
       <c r="N225" s="3">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="O225" s="29">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="P225" s="18">
         <v>0</v>
       </c>
       <c r="Q225" s="2" t="s">
-        <v>1251</v>
+        <v>1232</v>
       </c>
       <c r="R225" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="S225" s="20">
-        <v>300000</v>
+        <v>100000</v>
       </c>
       <c r="T225" s="31">
         <v>0</v>
@@ -32300,6 +32319,237 @@
       </c>
       <c r="Y225" s="43">
         <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A226" s="13" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B226" s="13" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C226" s="13" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D226" s="23">
+        <v>40</v>
+      </c>
+      <c r="E226" s="33">
+        <v>400000</v>
+      </c>
+      <c r="F226" s="35">
+        <v>400000</v>
+      </c>
+      <c r="G226" s="41">
+        <v>150</v>
+      </c>
+      <c r="H226" s="25">
+        <v>90</v>
+      </c>
+      <c r="I226" s="24">
+        <v>10</v>
+      </c>
+      <c r="J226" s="34">
+        <v>200</v>
+      </c>
+      <c r="K226" s="26">
+        <v>0</v>
+      </c>
+      <c r="L226" s="27">
+        <v>1000</v>
+      </c>
+      <c r="M226" s="17">
+        <v>50</v>
+      </c>
+      <c r="N226" s="3">
+        <v>100</v>
+      </c>
+      <c r="O226" s="29">
+        <v>0</v>
+      </c>
+      <c r="P226" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q226" s="2" t="s">
+        <v>1273</v>
+      </c>
+      <c r="R226" t="s">
+        <v>1254</v>
+      </c>
+      <c r="S226" s="20">
+        <v>200000</v>
+      </c>
+      <c r="T226" s="31">
+        <v>0</v>
+      </c>
+      <c r="U226" s="38">
+        <v>0</v>
+      </c>
+      <c r="V226" s="36">
+        <v>0</v>
+      </c>
+      <c r="W226" s="47" t="s">
+        <v>668</v>
+      </c>
+      <c r="X226" s="57">
+        <v>1</v>
+      </c>
+      <c r="Y226" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A227" s="13" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B227" s="13" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C227" s="13" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D227" s="23">
+        <v>45</v>
+      </c>
+      <c r="E227" s="33">
+        <v>800000</v>
+      </c>
+      <c r="F227" s="35">
+        <v>800000</v>
+      </c>
+      <c r="G227" s="41">
+        <v>200</v>
+      </c>
+      <c r="H227" s="25">
+        <v>90</v>
+      </c>
+      <c r="I227" s="24">
+        <v>10</v>
+      </c>
+      <c r="J227" s="34">
+        <v>200</v>
+      </c>
+      <c r="K227" s="26">
+        <v>0</v>
+      </c>
+      <c r="L227" s="27">
+        <v>2000</v>
+      </c>
+      <c r="M227" s="17">
+        <v>100</v>
+      </c>
+      <c r="N227" s="3">
+        <v>75</v>
+      </c>
+      <c r="O227" s="29">
+        <v>75</v>
+      </c>
+      <c r="P227" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q227" s="2" t="s">
+        <v>1251</v>
+      </c>
+      <c r="R227" t="s">
+        <v>1255</v>
+      </c>
+      <c r="S227" s="20">
+        <v>300000</v>
+      </c>
+      <c r="T227" s="31">
+        <v>0</v>
+      </c>
+      <c r="U227" s="38">
+        <v>0</v>
+      </c>
+      <c r="V227" s="36">
+        <v>0</v>
+      </c>
+      <c r="W227" s="47" t="s">
+        <v>668</v>
+      </c>
+      <c r="X227" s="57">
+        <v>1</v>
+      </c>
+      <c r="Y227" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A228" s="13" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B228" s="13" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C228" s="13" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D228" s="23">
+        <v>60</v>
+      </c>
+      <c r="E228" s="33">
+        <v>1000000</v>
+      </c>
+      <c r="F228" s="35">
+        <v>1000000</v>
+      </c>
+      <c r="G228" s="41">
+        <v>400</v>
+      </c>
+      <c r="H228" s="25">
+        <v>70</v>
+      </c>
+      <c r="I228" s="24">
+        <v>1</v>
+      </c>
+      <c r="J228" s="34">
+        <v>200</v>
+      </c>
+      <c r="K228" s="26">
+        <v>25</v>
+      </c>
+      <c r="L228" s="27">
+        <v>5000</v>
+      </c>
+      <c r="M228" s="17">
+        <v>99</v>
+      </c>
+      <c r="N228" s="3">
+        <v>90</v>
+      </c>
+      <c r="O228" s="29">
+        <v>95</v>
+      </c>
+      <c r="P228" s="18">
+        <v>98</v>
+      </c>
+      <c r="Q228" s="2" t="s">
+        <v>1284</v>
+      </c>
+      <c r="R228" t="s">
+        <v>146</v>
+      </c>
+      <c r="S228" s="20">
+        <v>-1</v>
+      </c>
+      <c r="T228" s="31">
+        <v>0</v>
+      </c>
+      <c r="U228" s="38">
+        <v>1</v>
+      </c>
+      <c r="V228" s="36">
+        <v>0</v>
+      </c>
+      <c r="W228" s="47" t="s">
+        <v>1285</v>
+      </c>
+      <c r="X228" s="57">
+        <v>0</v>
+      </c>
+      <c r="Y228" s="43">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -32321,8 +32571,8 @@
   </sheetPr>
   <dimension ref="A1:J154"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J154"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Lair of the Magi blueprint
</commit_message>
<xml_diff>
--- a/data/Data Spreadsheet.xlsx
+++ b/data/Data Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="4"/>
+    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EXP" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3332" uniqueCount="1306">
   <si>
     <t>Club</t>
   </si>
@@ -3905,6 +3905,45 @@
   </si>
   <si>
     <t>Ugly Disguise</t>
+  </si>
+  <si>
+    <t>Undead Magus</t>
+  </si>
+  <si>
+    <t>Death Magus</t>
+  </si>
+  <si>
+    <t>Time Wizard</t>
+  </si>
+  <si>
+    <t>Henchman</t>
+  </si>
+  <si>
+    <t>Conjurer</t>
+  </si>
+  <si>
+    <t>Death Warrior</t>
+  </si>
+  <si>
+    <t>Fire Zealot</t>
+  </si>
+  <si>
+    <t>Abomination</t>
+  </si>
+  <si>
+    <t>Conjured Demon</t>
+  </si>
+  <si>
+    <t>Wonnen Daztinque</t>
+  </si>
+  <si>
+    <t>Touin DePenk</t>
+  </si>
+  <si>
+    <t>Arcane Sorcerer</t>
+  </si>
+  <si>
+    <t>Magus Wraith</t>
   </si>
 </sst>
 </file>
@@ -5091,11 +5130,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113945216"/>
-        <c:axId val="113947008"/>
+        <c:axId val="115518080"/>
+        <c:axId val="115519872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113945216"/>
+        <c:axId val="115518080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5105,7 +5144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113947008"/>
+        <c:crossAx val="115519872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5113,7 +5152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113947008"/>
+        <c:axId val="115519872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000"/>
@@ -5125,7 +5164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113945216"/>
+        <c:crossAx val="115518080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5816,11 +5855,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115041024"/>
-        <c:axId val="115042944"/>
+        <c:axId val="115565312"/>
+        <c:axId val="115567232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115041024"/>
+        <c:axId val="115565312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5848,7 +5887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115042944"/>
+        <c:crossAx val="115567232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5858,7 +5897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115042944"/>
+        <c:axId val="115567232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5869,7 +5908,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115041024"/>
+        <c:crossAx val="115565312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12721,7 +12760,7 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15029,13 +15068,13 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Y229"/>
+  <dimension ref="A1:Y242"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E186" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E193" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P228" sqref="P228"/>
+      <selection pane="bottomRight" activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32698,6 +32737,1007 @@
         <v>0</v>
       </c>
       <c r="Y229" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A230" s="13" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B230" s="13" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C230" s="13" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D230" s="23">
+        <v>0</v>
+      </c>
+      <c r="E230" s="33">
+        <v>0</v>
+      </c>
+      <c r="F230" s="35">
+        <v>0</v>
+      </c>
+      <c r="G230" s="41">
+        <v>0</v>
+      </c>
+      <c r="H230" s="25">
+        <v>0</v>
+      </c>
+      <c r="I230" s="24">
+        <v>0</v>
+      </c>
+      <c r="J230" s="34">
+        <v>0</v>
+      </c>
+      <c r="K230" s="26">
+        <v>0</v>
+      </c>
+      <c r="L230" s="27">
+        <v>0</v>
+      </c>
+      <c r="M230" s="17">
+        <v>0</v>
+      </c>
+      <c r="N230" s="3">
+        <v>0</v>
+      </c>
+      <c r="O230" s="29">
+        <v>0</v>
+      </c>
+      <c r="P230" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q230" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R230" t="s">
+        <v>146</v>
+      </c>
+      <c r="S230" s="20">
+        <v>0</v>
+      </c>
+      <c r="T230" s="31">
+        <v>0</v>
+      </c>
+      <c r="U230" s="38">
+        <v>1</v>
+      </c>
+      <c r="V230" s="36">
+        <v>0</v>
+      </c>
+      <c r="W230" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X230" s="57">
+        <v>0</v>
+      </c>
+      <c r="Y230" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A231" s="13" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B231" s="13" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C231" s="13" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D231" s="23">
+        <v>0</v>
+      </c>
+      <c r="E231" s="33">
+        <v>0</v>
+      </c>
+      <c r="F231" s="35">
+        <v>0</v>
+      </c>
+      <c r="G231" s="41">
+        <v>0</v>
+      </c>
+      <c r="H231" s="25">
+        <v>0</v>
+      </c>
+      <c r="I231" s="24">
+        <v>0</v>
+      </c>
+      <c r="J231" s="34">
+        <v>0</v>
+      </c>
+      <c r="K231" s="26">
+        <v>0</v>
+      </c>
+      <c r="L231" s="27">
+        <v>0</v>
+      </c>
+      <c r="M231" s="17">
+        <v>0</v>
+      </c>
+      <c r="N231" s="3">
+        <v>0</v>
+      </c>
+      <c r="O231" s="29">
+        <v>0</v>
+      </c>
+      <c r="P231" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q231" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R231" t="s">
+        <v>146</v>
+      </c>
+      <c r="S231" s="20">
+        <v>0</v>
+      </c>
+      <c r="T231" s="31">
+        <v>0</v>
+      </c>
+      <c r="U231" s="38">
+        <v>1</v>
+      </c>
+      <c r="V231" s="36">
+        <v>0</v>
+      </c>
+      <c r="W231" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X231" s="57">
+        <v>0</v>
+      </c>
+      <c r="Y231" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A232" s="13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B232" s="13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C232" s="13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D232" s="23">
+        <v>0</v>
+      </c>
+      <c r="E232" s="33">
+        <v>0</v>
+      </c>
+      <c r="F232" s="35">
+        <v>0</v>
+      </c>
+      <c r="G232" s="41">
+        <v>0</v>
+      </c>
+      <c r="H232" s="25">
+        <v>0</v>
+      </c>
+      <c r="I232" s="24">
+        <v>0</v>
+      </c>
+      <c r="J232" s="34">
+        <v>0</v>
+      </c>
+      <c r="K232" s="26">
+        <v>0</v>
+      </c>
+      <c r="L232" s="27">
+        <v>0</v>
+      </c>
+      <c r="M232" s="17">
+        <v>0</v>
+      </c>
+      <c r="N232" s="3">
+        <v>0</v>
+      </c>
+      <c r="O232" s="29">
+        <v>0</v>
+      </c>
+      <c r="P232" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q232" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R232" t="s">
+        <v>146</v>
+      </c>
+      <c r="S232" s="20">
+        <v>0</v>
+      </c>
+      <c r="T232" s="31">
+        <v>0</v>
+      </c>
+      <c r="U232" s="38">
+        <v>1</v>
+      </c>
+      <c r="V232" s="36">
+        <v>0</v>
+      </c>
+      <c r="W232" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X232" s="57">
+        <v>1</v>
+      </c>
+      <c r="Y232" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A233" s="13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B233" s="13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C233" s="13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D233" s="23">
+        <v>0</v>
+      </c>
+      <c r="E233" s="33">
+        <v>0</v>
+      </c>
+      <c r="F233" s="35">
+        <v>0</v>
+      </c>
+      <c r="G233" s="41">
+        <v>0</v>
+      </c>
+      <c r="H233" s="25">
+        <v>0</v>
+      </c>
+      <c r="I233" s="24">
+        <v>0</v>
+      </c>
+      <c r="J233" s="34">
+        <v>0</v>
+      </c>
+      <c r="K233" s="26">
+        <v>0</v>
+      </c>
+      <c r="L233" s="27">
+        <v>0</v>
+      </c>
+      <c r="M233" s="17">
+        <v>0</v>
+      </c>
+      <c r="N233" s="3">
+        <v>0</v>
+      </c>
+      <c r="O233" s="29">
+        <v>0</v>
+      </c>
+      <c r="P233" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q233" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R233" t="s">
+        <v>146</v>
+      </c>
+      <c r="S233" s="20">
+        <v>0</v>
+      </c>
+      <c r="T233" s="31">
+        <v>0</v>
+      </c>
+      <c r="U233" s="38">
+        <v>1</v>
+      </c>
+      <c r="V233" s="36">
+        <v>0</v>
+      </c>
+      <c r="W233" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X233" s="57">
+        <v>2</v>
+      </c>
+      <c r="Y233" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A234" s="13" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B234" s="13" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C234" s="13" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D234" s="23">
+        <v>0</v>
+      </c>
+      <c r="E234" s="33">
+        <v>0</v>
+      </c>
+      <c r="F234" s="35">
+        <v>0</v>
+      </c>
+      <c r="G234" s="41">
+        <v>0</v>
+      </c>
+      <c r="H234" s="25">
+        <v>0</v>
+      </c>
+      <c r="I234" s="24">
+        <v>0</v>
+      </c>
+      <c r="J234" s="34">
+        <v>0</v>
+      </c>
+      <c r="K234" s="26">
+        <v>0</v>
+      </c>
+      <c r="L234" s="27">
+        <v>0</v>
+      </c>
+      <c r="M234" s="17">
+        <v>0</v>
+      </c>
+      <c r="N234" s="3">
+        <v>0</v>
+      </c>
+      <c r="O234" s="29">
+        <v>0</v>
+      </c>
+      <c r="P234" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q234" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R234" t="s">
+        <v>146</v>
+      </c>
+      <c r="S234" s="20">
+        <v>0</v>
+      </c>
+      <c r="T234" s="31">
+        <v>0</v>
+      </c>
+      <c r="U234" s="38">
+        <v>1</v>
+      </c>
+      <c r="V234" s="36">
+        <v>0</v>
+      </c>
+      <c r="W234" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X234" s="57">
+        <v>3</v>
+      </c>
+      <c r="Y234" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A235" s="13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B235" s="13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C235" s="13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D235" s="23">
+        <v>0</v>
+      </c>
+      <c r="E235" s="33">
+        <v>0</v>
+      </c>
+      <c r="F235" s="35">
+        <v>0</v>
+      </c>
+      <c r="G235" s="41">
+        <v>0</v>
+      </c>
+      <c r="H235" s="25">
+        <v>0</v>
+      </c>
+      <c r="I235" s="24">
+        <v>0</v>
+      </c>
+      <c r="J235" s="34">
+        <v>0</v>
+      </c>
+      <c r="K235" s="26">
+        <v>0</v>
+      </c>
+      <c r="L235" s="27">
+        <v>0</v>
+      </c>
+      <c r="M235" s="17">
+        <v>0</v>
+      </c>
+      <c r="N235" s="3">
+        <v>0</v>
+      </c>
+      <c r="O235" s="29">
+        <v>0</v>
+      </c>
+      <c r="P235" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q235" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R235" t="s">
+        <v>146</v>
+      </c>
+      <c r="S235" s="20">
+        <v>0</v>
+      </c>
+      <c r="T235" s="31">
+        <v>0</v>
+      </c>
+      <c r="U235" s="38">
+        <v>1</v>
+      </c>
+      <c r="V235" s="36">
+        <v>0</v>
+      </c>
+      <c r="W235" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X235" s="57">
+        <v>4</v>
+      </c>
+      <c r="Y235" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A236" s="13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B236" s="13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C236" s="13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D236" s="23">
+        <v>0</v>
+      </c>
+      <c r="E236" s="33">
+        <v>0</v>
+      </c>
+      <c r="F236" s="35">
+        <v>0</v>
+      </c>
+      <c r="G236" s="41">
+        <v>0</v>
+      </c>
+      <c r="H236" s="25">
+        <v>0</v>
+      </c>
+      <c r="I236" s="24">
+        <v>0</v>
+      </c>
+      <c r="J236" s="34">
+        <v>0</v>
+      </c>
+      <c r="K236" s="26">
+        <v>0</v>
+      </c>
+      <c r="L236" s="27">
+        <v>0</v>
+      </c>
+      <c r="M236" s="17">
+        <v>0</v>
+      </c>
+      <c r="N236" s="3">
+        <v>0</v>
+      </c>
+      <c r="O236" s="29">
+        <v>0</v>
+      </c>
+      <c r="P236" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q236" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R236" t="s">
+        <v>146</v>
+      </c>
+      <c r="S236" s="20">
+        <v>0</v>
+      </c>
+      <c r="T236" s="31">
+        <v>0</v>
+      </c>
+      <c r="U236" s="38">
+        <v>1</v>
+      </c>
+      <c r="V236" s="36">
+        <v>0</v>
+      </c>
+      <c r="W236" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X236" s="57">
+        <v>5</v>
+      </c>
+      <c r="Y236" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A237" s="13" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B237" s="13" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C237" s="13" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D237" s="23">
+        <v>0</v>
+      </c>
+      <c r="E237" s="33">
+        <v>0</v>
+      </c>
+      <c r="F237" s="35">
+        <v>0</v>
+      </c>
+      <c r="G237" s="41">
+        <v>0</v>
+      </c>
+      <c r="H237" s="25">
+        <v>0</v>
+      </c>
+      <c r="I237" s="24">
+        <v>0</v>
+      </c>
+      <c r="J237" s="34">
+        <v>0</v>
+      </c>
+      <c r="K237" s="26">
+        <v>0</v>
+      </c>
+      <c r="L237" s="27">
+        <v>0</v>
+      </c>
+      <c r="M237" s="17">
+        <v>0</v>
+      </c>
+      <c r="N237" s="3">
+        <v>0</v>
+      </c>
+      <c r="O237" s="29">
+        <v>0</v>
+      </c>
+      <c r="P237" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q237" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R237" t="s">
+        <v>146</v>
+      </c>
+      <c r="S237" s="20">
+        <v>0</v>
+      </c>
+      <c r="T237" s="31">
+        <v>0</v>
+      </c>
+      <c r="U237" s="38">
+        <v>1</v>
+      </c>
+      <c r="V237" s="36">
+        <v>0</v>
+      </c>
+      <c r="W237" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X237" s="57">
+        <v>6</v>
+      </c>
+      <c r="Y237" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A238" s="13" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B238" s="13" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C238" s="13" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D238" s="23">
+        <v>0</v>
+      </c>
+      <c r="E238" s="33">
+        <v>0</v>
+      </c>
+      <c r="F238" s="35">
+        <v>0</v>
+      </c>
+      <c r="G238" s="41">
+        <v>0</v>
+      </c>
+      <c r="H238" s="25">
+        <v>0</v>
+      </c>
+      <c r="I238" s="24">
+        <v>0</v>
+      </c>
+      <c r="J238" s="34">
+        <v>0</v>
+      </c>
+      <c r="K238" s="26">
+        <v>0</v>
+      </c>
+      <c r="L238" s="27">
+        <v>0</v>
+      </c>
+      <c r="M238" s="17">
+        <v>0</v>
+      </c>
+      <c r="N238" s="3">
+        <v>0</v>
+      </c>
+      <c r="O238" s="29">
+        <v>0</v>
+      </c>
+      <c r="P238" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q238" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R238" t="s">
+        <v>146</v>
+      </c>
+      <c r="S238" s="20">
+        <v>0</v>
+      </c>
+      <c r="T238" s="31">
+        <v>0</v>
+      </c>
+      <c r="U238" s="38">
+        <v>1</v>
+      </c>
+      <c r="V238" s="36">
+        <v>0</v>
+      </c>
+      <c r="W238" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X238" s="57">
+        <v>7</v>
+      </c>
+      <c r="Y238" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A239" s="13" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B239" s="13" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C239" s="13" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D239" s="23">
+        <v>0</v>
+      </c>
+      <c r="E239" s="33">
+        <v>0</v>
+      </c>
+      <c r="F239" s="35">
+        <v>0</v>
+      </c>
+      <c r="G239" s="41">
+        <v>0</v>
+      </c>
+      <c r="H239" s="25">
+        <v>0</v>
+      </c>
+      <c r="I239" s="24">
+        <v>0</v>
+      </c>
+      <c r="J239" s="34">
+        <v>0</v>
+      </c>
+      <c r="K239" s="26">
+        <v>0</v>
+      </c>
+      <c r="L239" s="27">
+        <v>0</v>
+      </c>
+      <c r="M239" s="17">
+        <v>0</v>
+      </c>
+      <c r="N239" s="3">
+        <v>0</v>
+      </c>
+      <c r="O239" s="29">
+        <v>0</v>
+      </c>
+      <c r="P239" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q239" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R239" t="s">
+        <v>146</v>
+      </c>
+      <c r="S239" s="20">
+        <v>0</v>
+      </c>
+      <c r="T239" s="31">
+        <v>0</v>
+      </c>
+      <c r="U239" s="38">
+        <v>1</v>
+      </c>
+      <c r="V239" s="36">
+        <v>0</v>
+      </c>
+      <c r="W239" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X239" s="57">
+        <v>8</v>
+      </c>
+      <c r="Y239" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A240" s="13" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B240" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C240" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D240" s="23">
+        <v>0</v>
+      </c>
+      <c r="E240" s="33">
+        <v>0</v>
+      </c>
+      <c r="F240" s="35">
+        <v>0</v>
+      </c>
+      <c r="G240" s="41">
+        <v>0</v>
+      </c>
+      <c r="H240" s="25">
+        <v>0</v>
+      </c>
+      <c r="I240" s="24">
+        <v>0</v>
+      </c>
+      <c r="J240" s="34">
+        <v>0</v>
+      </c>
+      <c r="K240" s="26">
+        <v>0</v>
+      </c>
+      <c r="L240" s="27">
+        <v>0</v>
+      </c>
+      <c r="M240" s="17">
+        <v>0</v>
+      </c>
+      <c r="N240" s="3">
+        <v>0</v>
+      </c>
+      <c r="O240" s="29">
+        <v>0</v>
+      </c>
+      <c r="P240" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q240" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R240" t="s">
+        <v>146</v>
+      </c>
+      <c r="S240" s="20">
+        <v>0</v>
+      </c>
+      <c r="T240" s="31">
+        <v>0</v>
+      </c>
+      <c r="U240" s="38">
+        <v>1</v>
+      </c>
+      <c r="V240" s="36">
+        <v>0</v>
+      </c>
+      <c r="W240" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X240" s="57">
+        <v>9</v>
+      </c>
+      <c r="Y240" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A241" s="13" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B241" s="13" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C241" s="13" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D241" s="23">
+        <v>0</v>
+      </c>
+      <c r="E241" s="33">
+        <v>0</v>
+      </c>
+      <c r="F241" s="35">
+        <v>0</v>
+      </c>
+      <c r="G241" s="41">
+        <v>0</v>
+      </c>
+      <c r="H241" s="25">
+        <v>0</v>
+      </c>
+      <c r="I241" s="24">
+        <v>0</v>
+      </c>
+      <c r="J241" s="34">
+        <v>0</v>
+      </c>
+      <c r="K241" s="26">
+        <v>0</v>
+      </c>
+      <c r="L241" s="27">
+        <v>0</v>
+      </c>
+      <c r="M241" s="17">
+        <v>0</v>
+      </c>
+      <c r="N241" s="3">
+        <v>0</v>
+      </c>
+      <c r="O241" s="29">
+        <v>0</v>
+      </c>
+      <c r="P241" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q241" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R241" t="s">
+        <v>146</v>
+      </c>
+      <c r="S241" s="20">
+        <v>0</v>
+      </c>
+      <c r="T241" s="31">
+        <v>0</v>
+      </c>
+      <c r="U241" s="38">
+        <v>1</v>
+      </c>
+      <c r="V241" s="36">
+        <v>2</v>
+      </c>
+      <c r="W241" s="47" t="s">
+        <v>666</v>
+      </c>
+      <c r="X241" s="57">
+        <v>1</v>
+      </c>
+      <c r="Y241" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A242" s="13" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B242" s="13" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C242" s="13" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D242" s="23">
+        <v>0</v>
+      </c>
+      <c r="E242" s="33">
+        <v>0</v>
+      </c>
+      <c r="F242" s="35">
+        <v>0</v>
+      </c>
+      <c r="G242" s="41">
+        <v>0</v>
+      </c>
+      <c r="H242" s="25">
+        <v>0</v>
+      </c>
+      <c r="I242" s="24">
+        <v>0</v>
+      </c>
+      <c r="J242" s="34">
+        <v>0</v>
+      </c>
+      <c r="K242" s="26">
+        <v>0</v>
+      </c>
+      <c r="L242" s="27">
+        <v>0</v>
+      </c>
+      <c r="M242" s="17">
+        <v>0</v>
+      </c>
+      <c r="N242" s="3">
+        <v>0</v>
+      </c>
+      <c r="O242" s="29">
+        <v>0</v>
+      </c>
+      <c r="P242" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q242" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R242" t="s">
+        <v>146</v>
+      </c>
+      <c r="S242" s="20">
+        <v>0</v>
+      </c>
+      <c r="T242" s="31">
+        <v>0</v>
+      </c>
+      <c r="U242" s="38">
+        <v>1</v>
+      </c>
+      <c r="V242" s="36">
+        <v>1</v>
+      </c>
+      <c r="W242" s="47" t="s">
+        <v>666</v>
+      </c>
+      <c r="X242" s="57">
+        <v>1</v>
+      </c>
+      <c r="Y242" s="43">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make improvements to Fartooq Hold
- Give Oracular Orb a separate tile
- Add a new monster to the orb tile
- Rename Ice Guardian for more name variation
- Make map colour more suitable
- Fix completion flag in Adriatic Sea
</commit_message>
<xml_diff>
--- a/data/Data Spreadsheet.xlsx
+++ b/data/Data Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="4"/>
+    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EXP" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3414" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3484" uniqueCount="1450">
   <si>
     <t>Club</t>
   </si>
@@ -3701,9 +3701,6 @@
     <t>{'Fireball': 30, 'Fire Claw': 20, 'Firestorm': 30, 'Immolation': 20}</t>
   </si>
   <si>
-    <t>{'Icicles': 40, 'Hailstorm': 30, 'Dive': 20, 'Strong Attack': 10}</t>
-  </si>
-  <si>
     <t>{'Firestorm': 10, 'Fireball': 30, 'Burning Mind': 10}</t>
   </si>
   <si>
@@ -3977,9 +3974,6 @@
     <t>{'Freezing Arrow': 9, 'Mist': 6, 'Swoop': 7}</t>
   </si>
   <si>
-    <t>{'Luminescent Barrier': 1, 'Ash Bow': 4}</t>
-  </si>
-  <si>
     <t>Pespozeor2</t>
   </si>
   <si>
@@ -4148,21 +4142,12 @@
     <t>Daniel Quest 3 Complete</t>
   </si>
   <si>
-    <t>Kill 2 Rumadan men for Bartender Daniel in Herceg Novi.</t>
-  </si>
-  <si>
     <t>Manhunt</t>
   </si>
   <si>
-    <t>Kill 1 Kotor Crab for Bartender Daniel in Herceg Novi.</t>
-  </si>
-  <si>
     <t>Feeling Crabby</t>
   </si>
   <si>
-    <t>Kill Dr. Grabh for Bartender Daniel in Herceg Novi.</t>
-  </si>
-  <si>
     <t>I Need a Doctor!</t>
   </si>
   <si>
@@ -4200,6 +4185,198 @@
   </si>
   <si>
     <t>Hopalong Boots</t>
+  </si>
+  <si>
+    <t>Kill 1 Orc for Bartender Adam in Mojkovac Valley.</t>
+  </si>
+  <si>
+    <t>Kill 5 Goblins for Bartender Adam in Mojkovac Valley.</t>
+  </si>
+  <si>
+    <t>Ice Elemental</t>
+  </si>
+  <si>
+    <t>Frozen Guardian</t>
+  </si>
+  <si>
+    <t>{'Icicles': 50, 'Hailstorm': 10, 'Dive': 20, 'Strong Attack': 10}</t>
+  </si>
+  <si>
+    <t>{'Icicles': 40, 'Hailstorm': 30, 'Healing Glow': 20, 'Rock Shot': 10}</t>
+  </si>
+  <si>
+    <t>{'Luminescent Barrier': 1, 'Ash Bow': 5}</t>
+  </si>
+  <si>
+    <t>{'Radiant Barrier': 15}</t>
+  </si>
+  <si>
+    <t>{'Wildcard Kills': (('Goblin', 'Mountain Goblin', 'Goblin Ranger', 'Goblin Thug'), 5, "Goblin")}</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Orc', 1)}</t>
+  </si>
+  <si>
+    <t>Kill 5 Giant Seals for Bartender Adam in Mojkovac Valley.</t>
+  </si>
+  <si>
+    <t>Adam Quest 2</t>
+  </si>
+  <si>
+    <t>Adam Quest 1</t>
+  </si>
+  <si>
+    <t>Adam Quest 3</t>
+  </si>
+  <si>
+    <t>Adam Quest 1 Complete</t>
+  </si>
+  <si>
+    <t>Adam Quest 2 Complete</t>
+  </si>
+  <si>
+    <t>Adam Quest 3 Complete</t>
+  </si>
+  <si>
+    <t>Sealing the Deal</t>
+  </si>
+  <si>
+    <t>A Cute Goblinhide Coat</t>
+  </si>
+  <si>
+    <t>A Lovely Orcskin Jacket</t>
+  </si>
+  <si>
+    <t>Rescue Dragan's father from inside The Watchmaking Facility.</t>
+  </si>
+  <si>
+    <t>Father Time</t>
+  </si>
+  <si>
+    <t>The Watchmaking Facility Complete</t>
+  </si>
+  <si>
+    <t>Ghost of Tomas Conclusion</t>
+  </si>
+  <si>
+    <t>Grave Matters</t>
+  </si>
+  <si>
+    <t>Bury Dragan's father in the cemetery.</t>
+  </si>
+  <si>
+    <t>Bartender Igor Quest 1</t>
+  </si>
+  <si>
+    <t>Bartender Igor Quest 2</t>
+  </si>
+  <si>
+    <t>Bartender Igor Quest 3</t>
+  </si>
+  <si>
+    <t>Bartender Igor Quest 1 Complete</t>
+  </si>
+  <si>
+    <t>Bartender Igor Quest 2 Complete</t>
+  </si>
+  <si>
+    <t>Bartender Igor Quest 3 Complete</t>
+  </si>
+  <si>
+    <t>Fresh or Fowl?</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Unholy Crow', 1)}</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Toxic Jellyfish', 3)}</t>
+  </si>
+  <si>
+    <t>Kill 1 crow for Bartender Igor in Pec.</t>
+  </si>
+  <si>
+    <t>Kill 3 jellyfish for Bartender Igor in Pec.</t>
+  </si>
+  <si>
+    <t>Kill 3 octopi for Bartender Igor in Pec.</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Mystical Octopus', 3)}</t>
+  </si>
+  <si>
+    <t>"Ate" Legged</t>
+  </si>
+  <si>
+    <t>A Shocking Choice</t>
+  </si>
+  <si>
+    <t>Bartender Zhang Quest 1</t>
+  </si>
+  <si>
+    <t>Bartender Zhang Quest 1 Complete</t>
+  </si>
+  <si>
+    <t>Bartender Zhang Quest 2</t>
+  </si>
+  <si>
+    <t>Bartender Zhang Quest 2 Complete</t>
+  </si>
+  <si>
+    <t>Bartender Zhang Quest 3</t>
+  </si>
+  <si>
+    <t>Bartender Zhang Quest 3 Complete</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Border Guard', 5)}</t>
+  </si>
+  <si>
+    <t>Kill 5 Border Guards for Bartender Zhang in Pristina.</t>
+  </si>
+  <si>
+    <t>Business as Usual</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Black Knight', 10)}</t>
+  </si>
+  <si>
+    <t>Kill 10 Black Knights for Bartender Zhang in Pristina.</t>
+  </si>
+  <si>
+    <t>{'Kills': ('General Octavius', 1)}</t>
+  </si>
+  <si>
+    <t>Continue your journey north through Black Mountain to reach Mojkovac.</t>
+  </si>
+  <si>
+    <t>Mojkovac Summit</t>
+  </si>
+  <si>
+    <t>Homeland Bound</t>
+  </si>
+  <si>
+    <t>Kill General Octavius for Bartender Zhang in Pristina. He can be found in a corner of Kosovo.</t>
+  </si>
+  <si>
+    <t>Kill 2 Rumadan men for Bartender Daniel in Herceg Novi. They can be found in the Frolicking Fields nearby.</t>
+  </si>
+  <si>
+    <t>Kill 1 Kotor Crab for Bartender Daniel in Herceg Novi. They can be found in the Bay of Kotor to the south.</t>
+  </si>
+  <si>
+    <t>Find and kill Dr. Grabh for Bartender Daniel in Herceg Novi.</t>
+  </si>
+  <si>
+    <t>Honey Rod</t>
+  </si>
+  <si>
+    <t>{'Kills': ('Giant Seal1', 5)}</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>Getting Medieval</t>
   </si>
 </sst>
 </file>
@@ -5386,11 +5563,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127036416"/>
-        <c:axId val="127992576"/>
+        <c:axId val="127630336"/>
+        <c:axId val="127660800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127036416"/>
+        <c:axId val="127630336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5400,7 +5577,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127992576"/>
+        <c:crossAx val="127660800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5408,7 +5585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127992576"/>
+        <c:axId val="127660800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000"/>
@@ -5420,7 +5597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127036416"/>
+        <c:crossAx val="127630336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7432,8 +7609,8 @@
   <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8952,7 +9129,7 @@
     </row>
     <row r="48" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="64" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B48" s="64" t="s">
         <v>171</v>
@@ -12208,7 +12385,7 @@
         <v>146</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="J149" s="2" t="s">
         <v>155</v>
@@ -12240,7 +12417,7 @@
         <v>146</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="J150" s="2" t="s">
         <v>155</v>
@@ -12272,7 +12449,7 @@
         <v>146</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="J151" s="2" t="s">
         <v>155</v>
@@ -12280,7 +12457,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B152" t="s">
         <v>249</v>
@@ -12304,15 +12481,15 @@
         <v>146</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B153" t="s">
         <v>157</v>
@@ -12327,7 +12504,7 @@
         <v>200</v>
       </c>
       <c r="F153" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>146</v>
@@ -12336,7 +12513,7 @@
         <v>146</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="J153" s="2" t="s">
         <v>155</v>
@@ -12344,7 +12521,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B154" t="s">
         <v>176</v>
@@ -12359,7 +12536,7 @@
         <v>300</v>
       </c>
       <c r="F154" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="G154" t="s">
         <v>146</v>
@@ -12368,7 +12545,7 @@
         <v>640</v>
       </c>
       <c r="I154" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="J154" t="s">
         <v>155</v>
@@ -12376,10 +12553,10 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="B155" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="C155" t="s">
         <v>159</v>
@@ -12400,7 +12577,7 @@
         <v>146</v>
       </c>
       <c r="I155" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="J155" t="s">
         <v>155</v>
@@ -16296,11 +16473,11 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="A1:I61"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16745,28 +16922,28 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>1446</v>
       </c>
       <c r="B16" s="43">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="C16" t="s">
         <v>124</v>
       </c>
       <c r="D16">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E16" s="46">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="H16">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="I16">
         <v>200</v>
@@ -16774,28 +16951,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="43">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="C17" t="s">
         <v>124</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E17" s="46">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
         <v>125</v>
       </c>
       <c r="G17" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I17">
         <v>200</v>
@@ -16803,28 +16980,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="43">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="C18" t="s">
         <v>124</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E18" s="46">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="I18">
         <v>200</v>
@@ -16832,28 +17009,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="43">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="C19" t="s">
         <v>124</v>
       </c>
       <c r="D19">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E19" s="46">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G19" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H19">
-        <v>8</v>
+        <v>0.1</v>
       </c>
       <c r="I19">
         <v>200</v>
@@ -16861,25 +17038,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B20" s="43">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="C20" t="s">
         <v>124</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E20" s="46">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
         <v>125</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H20">
         <v>8</v>
@@ -16890,28 +17067,28 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B21" s="43">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="C21" t="s">
         <v>124</v>
       </c>
       <c r="D21">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E21" s="46">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H21">
-        <v>6.8</v>
+        <v>8</v>
       </c>
       <c r="I21">
         <v>200</v>
@@ -16919,28 +17096,28 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="43">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="C22" t="s">
         <v>124</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E22" s="46">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>6.8</v>
       </c>
       <c r="I22">
         <v>200</v>
@@ -16948,28 +17125,28 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="43">
-        <v>2400</v>
+        <v>200</v>
       </c>
       <c r="C23" t="s">
         <v>124</v>
       </c>
       <c r="D23">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E23" s="46">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H23">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="I23">
         <v>200</v>
@@ -16977,10 +17154,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="43">
-        <v>900</v>
+        <v>2400</v>
       </c>
       <c r="C24" t="s">
         <v>124</v>
@@ -16989,16 +17166,16 @@
         <v>50</v>
       </c>
       <c r="E24" s="46">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G24" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H24">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="I24">
         <v>200</v>
@@ -17006,28 +17183,28 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="43">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="D25">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E25" s="46">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G25" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="I25">
         <v>200</v>
@@ -17035,28 +17212,28 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="43">
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
       <c r="D26">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E26" s="46">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H26">
-        <v>6</v>
+        <v>0.1</v>
       </c>
       <c r="I26">
         <v>200</v>
@@ -17064,28 +17241,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="43">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="C27" t="s">
         <v>124</v>
       </c>
       <c r="D27">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E27" s="46">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
         <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I27">
         <v>200</v>
@@ -17093,28 +17270,28 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="43">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="C28" t="s">
         <v>124</v>
       </c>
       <c r="D28">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E28" s="46">
         <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H28">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="I28">
         <v>200</v>
@@ -17122,86 +17299,86 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="43">
-        <v>4000</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1236</v>
+        <v>2000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
       </c>
       <c r="D29">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E29" s="46">
         <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>7.2</v>
       </c>
       <c r="I29">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="43">
-        <v>7777</v>
-      </c>
-      <c r="C30" t="s">
-        <v>124</v>
+        <v>4000</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>1235</v>
       </c>
       <c r="D30">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="E30" s="46">
         <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G30" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="43">
-        <v>1500</v>
+        <v>7777</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="D31">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E31" s="46">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G31" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>200</v>
@@ -17209,28 +17386,28 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="43">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="D32">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="E32" s="46">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F32" t="s">
         <v>125</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I32">
         <v>200</v>
@@ -17238,28 +17415,28 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="43">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="C33" t="s">
         <v>124</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="E33" s="46">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="F33" t="s">
         <v>125</v>
       </c>
       <c r="G33" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I33">
         <v>200</v>
@@ -17267,28 +17444,28 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>677</v>
+        <v>37</v>
       </c>
       <c r="B34" s="43">
-        <v>3800</v>
+        <v>1800</v>
       </c>
       <c r="C34" t="s">
         <v>124</v>
       </c>
       <c r="D34">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="E34" s="46">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="F34" t="s">
         <v>125</v>
       </c>
       <c r="G34" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H34">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I34">
         <v>200</v>
@@ -17296,28 +17473,28 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>677</v>
       </c>
       <c r="B35" s="43">
-        <v>3600</v>
+        <v>3800</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="D35">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E35" s="46">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
         <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I35">
         <v>200</v>
@@ -17325,28 +17502,28 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1174</v>
+        <v>38</v>
       </c>
       <c r="B36" s="43">
-        <v>4699</v>
+        <v>3600</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="D36">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E36" s="46">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H36">
-        <v>7.6</v>
+        <v>6</v>
       </c>
       <c r="I36">
         <v>200</v>
@@ -17354,10 +17531,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>1174</v>
       </c>
       <c r="B37" s="43">
-        <v>4000</v>
+        <v>4699</v>
       </c>
       <c r="C37" t="s">
         <v>124</v>
@@ -17366,7 +17543,7 @@
         <v>80</v>
       </c>
       <c r="E37" s="46">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F37" t="s">
         <v>126</v>
@@ -17383,28 +17560,28 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="43">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C38" t="s">
         <v>124</v>
       </c>
       <c r="D38">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E38" s="46">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G38" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>7.6</v>
       </c>
       <c r="I38">
         <v>200</v>
@@ -17412,28 +17589,28 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1172</v>
+        <v>41</v>
       </c>
       <c r="B39" s="43">
-        <v>4699</v>
+        <v>5000</v>
       </c>
       <c r="C39" t="s">
         <v>124</v>
       </c>
       <c r="D39">
+        <v>60</v>
+      </c>
+      <c r="E39" s="46">
         <v>65</v>
-      </c>
-      <c r="E39" s="46">
-        <v>58</v>
       </c>
       <c r="F39" t="s">
         <v>125</v>
       </c>
       <c r="G39" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H39">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I39">
         <v>200</v>
@@ -17441,10 +17618,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>1172</v>
       </c>
       <c r="B40" s="43">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="C40" t="s">
         <v>124</v>
@@ -17453,7 +17630,7 @@
         <v>65</v>
       </c>
       <c r="E40" s="46">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F40" t="s">
         <v>125</v>
@@ -17470,28 +17647,28 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1173</v>
+        <v>42</v>
       </c>
       <c r="B41" s="43">
-        <v>4699</v>
+        <v>4700</v>
       </c>
       <c r="C41" t="s">
         <v>124</v>
       </c>
       <c r="D41">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E41" s="46">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G41" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="I41">
         <v>200</v>
@@ -17499,10 +17676,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>717</v>
+        <v>1173</v>
       </c>
       <c r="B42" s="43">
-        <v>4800</v>
+        <v>4699</v>
       </c>
       <c r="C42" t="s">
         <v>124</v>
@@ -17511,7 +17688,7 @@
         <v>70</v>
       </c>
       <c r="E42" s="46">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F42" t="s">
         <v>127</v>
@@ -17528,28 +17705,28 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>717</v>
       </c>
       <c r="B43" s="43">
-        <v>4700</v>
+        <v>4800</v>
       </c>
       <c r="C43" t="s">
         <v>124</v>
       </c>
       <c r="D43">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E43" s="46">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F43" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H43">
-        <v>8</v>
+        <v>0.1</v>
       </c>
       <c r="I43">
         <v>200</v>
@@ -17557,25 +17734,25 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="43">
-        <v>4500</v>
+        <v>4700</v>
       </c>
       <c r="C44" t="s">
         <v>124</v>
       </c>
       <c r="D44">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E44" s="46">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
         <v>125</v>
       </c>
       <c r="G44" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H44">
         <v>8</v>
@@ -17586,86 +17763,86 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="43">
-        <v>5000</v>
+        <v>4500</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="D45">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E45" s="46">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F45" t="s">
         <v>125</v>
       </c>
       <c r="G45" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H45">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="I45">
         <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>1265</v>
+      <c r="A46" t="s">
+        <v>45</v>
       </c>
       <c r="B46" s="43">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
       <c r="D46">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E46" s="46">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G46" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H46">
-        <v>0.1</v>
+        <v>30</v>
       </c>
       <c r="I46">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>477</v>
+      <c r="A47" s="2" t="s">
+        <v>1264</v>
       </c>
       <c r="B47" s="43">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="C47" t="s">
         <v>124</v>
       </c>
       <c r="D47">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E47" s="46">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F47" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G47" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H47">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="I47">
         <v>200</v>
@@ -17673,28 +17850,28 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1213</v>
+        <v>477</v>
       </c>
       <c r="B48" s="43">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="C48" t="s">
         <v>124</v>
       </c>
       <c r="D48">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E48" s="46">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F48" t="s">
         <v>125</v>
       </c>
       <c r="G48" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I48">
         <v>200</v>
@@ -17702,25 +17879,25 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>1213</v>
       </c>
       <c r="B49" s="43">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="C49" t="s">
         <v>124</v>
       </c>
       <c r="D49">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E49" s="46">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H49">
         <v>8</v>
@@ -17731,28 +17908,28 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" s="43">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E50" s="46">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F50" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G50" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I50">
         <v>200</v>
@@ -17760,28 +17937,28 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="43">
-        <v>7000</v>
+        <v>7500</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="D51">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E51" s="46">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F51" t="s">
         <v>125</v>
       </c>
       <c r="G51" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="H51">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I51">
         <v>200</v>
@@ -17789,7 +17966,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="43">
         <v>7000</v>
@@ -17801,16 +17978,16 @@
         <v>100</v>
       </c>
       <c r="E52" s="46">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
         <v>125</v>
       </c>
       <c r="G52" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H52">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I52">
         <v>200</v>
@@ -17818,7 +17995,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="43">
         <v>7000</v>
@@ -17830,16 +18007,16 @@
         <v>100</v>
       </c>
       <c r="E53" s="46">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F53" t="s">
         <v>125</v>
       </c>
       <c r="G53" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H53">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I53">
         <v>200</v>
@@ -17847,7 +18024,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>986</v>
+        <v>50</v>
       </c>
       <c r="B54" s="43">
         <v>7000</v>
@@ -17859,16 +18036,16 @@
         <v>100</v>
       </c>
       <c r="E54" s="46">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F54" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G54" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="I54">
         <v>200</v>
@@ -17876,7 +18053,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>803</v>
+        <v>986</v>
       </c>
       <c r="B55" s="43">
         <v>7000</v>
@@ -17888,16 +18065,16 @@
         <v>100</v>
       </c>
       <c r="E55" s="46">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G55" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H55">
-        <v>6</v>
+        <v>0.1</v>
       </c>
       <c r="I55">
         <v>200</v>
@@ -17905,7 +18082,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>803</v>
       </c>
       <c r="B56" s="43">
         <v>7000</v>
@@ -17917,16 +18094,16 @@
         <v>100</v>
       </c>
       <c r="E56" s="46">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="F56" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G56" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I56">
         <v>200</v>
@@ -17934,19 +18111,19 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1243</v>
+        <v>51</v>
       </c>
       <c r="B57" s="43">
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="C57" t="s">
         <v>124</v>
       </c>
       <c r="D57">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E57" s="46">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F57" t="s">
         <v>125</v>
@@ -17955,65 +18132,65 @@
         <v>3</v>
       </c>
       <c r="H57">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I57">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>279</v>
+        <v>1242</v>
       </c>
       <c r="B58" s="43">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="C58" t="s">
         <v>124</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="E58" s="46">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="F58" t="s">
         <v>125</v>
       </c>
       <c r="G58" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I58">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1323</v>
+        <v>279</v>
       </c>
       <c r="B59" s="43">
-        <v>7000</v>
+        <v>0</v>
       </c>
       <c r="C59" t="s">
         <v>124</v>
       </c>
       <c r="D59">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E59" s="46">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G59" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="I59">
         <v>200</v>
@@ -18021,28 +18198,28 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="B60" s="43">
-        <v>7500</v>
+        <v>7000</v>
       </c>
       <c r="C60" t="s">
         <v>124</v>
       </c>
       <c r="D60">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="E60" s="46">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F60" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G60" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H60">
-        <v>12</v>
+        <v>0.1</v>
       </c>
       <c r="I60">
         <v>200</v>
@@ -18050,7 +18227,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="B61" s="43">
         <v>7500</v>
@@ -18059,21 +18236,50 @@
         <v>124</v>
       </c>
       <c r="D61">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E61" s="46">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F61" t="s">
         <v>125</v>
       </c>
       <c r="G61" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61">
+        <v>12</v>
+      </c>
+      <c r="I61">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B62" s="43">
+        <v>7500</v>
+      </c>
+      <c r="C62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62">
+        <v>111</v>
+      </c>
+      <c r="E62" s="46">
+        <v>81</v>
+      </c>
+      <c r="F62" t="s">
+        <v>125</v>
+      </c>
+      <c r="G62" t="s">
         <v>3</v>
       </c>
-      <c r="H61">
+      <c r="H62">
         <v>4</v>
       </c>
-      <c r="I61">
+      <c r="I62">
         <v>200</v>
       </c>
     </row>
@@ -18091,7 +18297,7 @@
   </sheetPr>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18860,7 +19066,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B39" s="43">
         <v>8000</v>
@@ -19060,7 +19266,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B49" s="43">
         <v>5000</v>
@@ -19080,7 +19286,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B50" s="43">
         <v>5000</v>
@@ -19100,7 +19306,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B51" s="43">
         <v>5000</v>
@@ -19120,7 +19326,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B52" s="43">
         <v>8000</v>
@@ -19140,7 +19346,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B53" s="43">
         <v>1225</v>
@@ -19160,7 +19366,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B54" s="43">
         <v>8000</v>
@@ -19180,7 +19386,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="B55" s="43">
         <v>8000</v>
@@ -19200,7 +19406,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1390</v>
+        <v>1385</v>
       </c>
       <c r="B56" s="43">
         <v>1225</v>
@@ -19234,7 +19440,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:G40"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19681,7 +19887,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B20" s="43">
         <v>3500</v>
@@ -19911,7 +20117,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B30" s="43">
         <v>8000</v>
@@ -20141,7 +20347,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="B40" s="43">
         <v>7000</v>
@@ -20335,7 +20541,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -20445,29 +20651,29 @@
         <v>0</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B21" s="43">
+        <v>0</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>1260</v>
-      </c>
-      <c r="B21" s="43">
-        <v>0</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>1261</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B22" s="43">
+        <v>0</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>1287</v>
-      </c>
-      <c r="B22" s="43">
-        <v>0</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>1288</v>
       </c>
     </row>
   </sheetData>
@@ -20480,17 +20686,17 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
@@ -20498,104 +20704,308 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C1" t="s">
         <v>1362</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1363</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1364</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1365</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1366</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1374</v>
+        <v>530</v>
       </c>
       <c r="B2" t="s">
-        <v>1373</v>
+        <v>1383</v>
       </c>
       <c r="C2" t="s">
-        <v>1379</v>
+        <v>1384</v>
       </c>
       <c r="D2" t="s">
-        <v>1367</v>
+        <v>697</v>
       </c>
       <c r="E2" t="s">
-        <v>1368</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1376</v>
+        <v>1371</v>
       </c>
       <c r="B3" t="s">
-        <v>1375</v>
+        <v>1443</v>
       </c>
       <c r="C3" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="D3" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="E3" t="s">
-        <v>1371</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="B4" t="s">
-        <v>1377</v>
+        <v>1444</v>
       </c>
       <c r="C4" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="D4" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="E4" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1386</v>
+        <v>1373</v>
       </c>
       <c r="B5" t="s">
-        <v>1385</v>
+        <v>1445</v>
       </c>
       <c r="C5" t="s">
-        <v>1384</v>
+        <v>1376</v>
       </c>
       <c r="D5" t="s">
-        <v>1383</v>
+        <v>1368</v>
       </c>
       <c r="E5" t="s">
-        <v>1382</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>530</v>
+        <v>1381</v>
       </c>
       <c r="B6" t="s">
-        <v>1388</v>
+        <v>1380</v>
       </c>
       <c r="C6" t="s">
-        <v>1389</v>
+        <v>1379</v>
       </c>
       <c r="D6" t="s">
-        <v>697</v>
+        <v>1378</v>
       </c>
       <c r="E6" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B8" t="s">
         <v>1387</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" t="s">
+        <v>411</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1409</v>
       </c>
     </row>
   </sheetData>
@@ -20608,13 +21018,13 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Y246"/>
+  <dimension ref="A1:Y247"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="R209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" sqref="A1:Y247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21777,7 +22187,7 @@
         <v>729</v>
       </c>
       <c r="R15" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S15" s="20">
         <v>50</v>
@@ -21851,10 +22261,10 @@
         <v>80</v>
       </c>
       <c r="Q16" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="R16" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="S16" s="20">
         <v>3700</v>
@@ -22162,7 +22572,7 @@
         <v>362</v>
       </c>
       <c r="R20" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="S20" s="20">
         <v>75</v>
@@ -22316,7 +22726,7 @@
         <v>366</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="S22" s="20">
         <v>75</v>
@@ -22855,7 +23265,7 @@
         <v>998</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="S29" s="21">
         <v>150</v>
@@ -23083,7 +23493,7 @@
         <v>0</v>
       </c>
       <c r="Q32" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="R32" t="s">
         <v>620</v>
@@ -23471,7 +23881,7 @@
         <v>487</v>
       </c>
       <c r="R37" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="S37" s="20">
         <v>230</v>
@@ -23933,7 +24343,7 @@
         <v>1001</v>
       </c>
       <c r="R43" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="S43" s="21">
         <v>280</v>
@@ -24164,7 +24574,7 @@
         <v>488</v>
       </c>
       <c r="R46" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="S46" s="20">
         <v>310</v>
@@ -24315,7 +24725,7 @@
         <v>0</v>
       </c>
       <c r="Q48" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="R48" t="s">
         <v>485</v>
@@ -24472,7 +24882,7 @@
         <v>608</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="S50" s="21">
         <v>360</v>
@@ -26859,7 +27269,7 @@
         <v>564</v>
       </c>
       <c r="R81" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="S81" s="20">
         <v>730</v>
@@ -27629,7 +28039,7 @@
         <v>808</v>
       </c>
       <c r="R91" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="S91" s="20">
         <v>900</v>
@@ -28165,7 +28575,7 @@
         <v>0</v>
       </c>
       <c r="Q98" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="R98" t="s">
         <v>849</v>
@@ -28704,7 +29114,7 @@
         <v>10</v>
       </c>
       <c r="Q105" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="R105" s="2" t="s">
         <v>1211</v>
@@ -29015,7 +29425,7 @@
         <v>995</v>
       </c>
       <c r="R109" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="S109" s="20">
         <v>1500</v>
@@ -29859,7 +30269,7 @@
         <v>0</v>
       </c>
       <c r="Q120" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="R120" t="s">
         <v>146</v>
@@ -34713,7 +35123,7 @@
         <v>1103</v>
       </c>
       <c r="R183" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="S183" s="20">
         <v>9000</v>
@@ -34790,7 +35200,7 @@
         <v>1119</v>
       </c>
       <c r="R184" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="S184" s="20">
         <v>9000</v>
@@ -34867,7 +35277,7 @@
         <v>1097</v>
       </c>
       <c r="R185" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="S185" s="20">
         <v>9000</v>
@@ -34944,7 +35354,7 @@
         <v>1088</v>
       </c>
       <c r="R186" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="S186" s="20">
         <v>8000</v>
@@ -35021,7 +35431,7 @@
         <v>1074</v>
       </c>
       <c r="R187" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="S187" s="20">
         <v>8000</v>
@@ -35098,7 +35508,7 @@
         <v>1159</v>
       </c>
       <c r="R188" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="S188" s="20">
         <v>8000</v>
@@ -35175,7 +35585,7 @@
         <v>1070</v>
       </c>
       <c r="R189" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="S189" s="20">
         <v>7000</v>
@@ -35252,7 +35662,7 @@
         <v>1068</v>
       </c>
       <c r="R190" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="S190" s="20">
         <v>7000</v>
@@ -35329,7 +35739,7 @@
         <v>1092</v>
       </c>
       <c r="R191" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="S191" s="20">
         <v>7000</v>
@@ -35406,7 +35816,7 @@
         <v>1158</v>
       </c>
       <c r="R192" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="S192" s="20">
         <v>6000</v>
@@ -35483,7 +35893,7 @@
         <v>1069</v>
       </c>
       <c r="R193" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="S193" s="20">
         <v>6000</v>
@@ -35560,7 +35970,7 @@
         <v>1059</v>
       </c>
       <c r="R194" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="S194" s="20">
         <v>6000</v>
@@ -35637,7 +36047,7 @@
         <v>1052</v>
       </c>
       <c r="R195" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="S195" s="20">
         <v>5000</v>
@@ -35714,7 +36124,7 @@
         <v>1051</v>
       </c>
       <c r="R196" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="S196" s="20">
         <v>5000</v>
@@ -35791,7 +36201,7 @@
         <v>1047</v>
       </c>
       <c r="R197" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="S197" s="20">
         <v>5000</v>
@@ -36022,7 +36432,7 @@
         <v>1149</v>
       </c>
       <c r="R200" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="S200" s="20">
         <v>30000</v>
@@ -36099,7 +36509,7 @@
         <v>1150</v>
       </c>
       <c r="R201" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="S201" s="20">
         <v>30000</v>
@@ -36279,13 +36689,13 @@
     </row>
     <row r="204" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A204" s="13" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="C204" s="13" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D204" s="23">
         <v>20</v>
@@ -36357,13 +36767,13 @@
     </row>
     <row r="205" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A205" s="13" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="C205" s="13" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D205" s="23">
         <v>4</v>
@@ -36434,13 +36844,13 @@
     </row>
     <row r="206" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A206" s="12" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>1255</v>
+        <v>1389</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D206" s="23">
         <v>30</v>
@@ -36482,7 +36892,7 @@
         <v>50</v>
       </c>
       <c r="Q206" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="R206" t="s">
         <v>1007</v>
@@ -36559,7 +36969,7 @@
         <v>100</v>
       </c>
       <c r="Q207" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="R207" t="s">
         <v>1193</v>
@@ -36636,7 +37046,7 @@
         <v>100</v>
       </c>
       <c r="Q208" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="R208" t="s">
         <v>1194</v>
@@ -36713,7 +37123,7 @@
         <v>100</v>
       </c>
       <c r="Q209" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="R209" t="s">
         <v>1195</v>
@@ -37098,7 +37508,7 @@
         <v>25</v>
       </c>
       <c r="Q214" t="s">
-        <v>1224</v>
+        <v>1390</v>
       </c>
       <c r="R214" t="s">
         <v>1209</v>
@@ -37204,13 +37614,13 @@
     </row>
     <row r="216" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A216" s="13" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B216" s="13" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C216" s="13" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="D216" s="23">
         <v>25</v>
@@ -37252,7 +37662,7 @@
         <v>0</v>
       </c>
       <c r="Q216" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="R216" t="s">
         <v>146</v>
@@ -37329,7 +37739,7 @@
         <v>0</v>
       </c>
       <c r="Q217" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="R217" t="s">
         <v>1220</v>
@@ -37483,10 +37893,10 @@
         <v>0</v>
       </c>
       <c r="Q219" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="R219" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="S219" s="20">
         <v>1300</v>
@@ -37512,13 +37922,13 @@
     </row>
     <row r="220" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A220" s="13" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C220" s="13" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="D220" s="23">
         <v>30</v>
@@ -37560,10 +37970,10 @@
         <v>50</v>
       </c>
       <c r="Q220" t="s">
+        <v>1275</v>
+      </c>
+      <c r="R220" t="s">
         <v>1276</v>
-      </c>
-      <c r="R220" t="s">
-        <v>1277</v>
       </c>
       <c r="S220" s="20">
         <v>1700</v>
@@ -37666,13 +38076,13 @@
     </row>
     <row r="222" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A222" s="13" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C222" s="13" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="D222" s="23">
         <v>30</v>
@@ -37714,10 +38124,10 @@
         <v>100</v>
       </c>
       <c r="Q222" s="2" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="R222" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="S222" s="20">
         <v>4000</v>
@@ -37820,13 +38230,13 @@
     </row>
     <row r="224" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A224" s="13" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C224" s="13" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="D224" s="23">
         <v>35</v>
@@ -37868,10 +38278,10 @@
         <v>99</v>
       </c>
       <c r="Q224" s="2" t="s">
+        <v>1277</v>
+      </c>
+      <c r="R224" s="2" t="s">
         <v>1278</v>
-      </c>
-      <c r="R224" s="2" t="s">
-        <v>1279</v>
       </c>
       <c r="S224" s="20">
         <v>9000</v>
@@ -37945,10 +38355,10 @@
         <v>0</v>
       </c>
       <c r="Q225" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="R225" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="S225" s="20">
         <v>100000</v>
@@ -38022,10 +38432,10 @@
         <v>0</v>
       </c>
       <c r="Q226" s="2" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="R226" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="S226" s="20">
         <v>200000</v>
@@ -38099,10 +38509,10 @@
         <v>0</v>
       </c>
       <c r="Q227" s="2" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="R227" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="S227" s="20">
         <v>300000</v>
@@ -38128,13 +38538,13 @@
     </row>
     <row r="228" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A228" s="12" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B228" t="s">
         <v>429</v>
       </c>
       <c r="C228" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="D228" s="23">
         <v>50</v>
@@ -38176,10 +38586,10 @@
         <v>25</v>
       </c>
       <c r="Q228" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="R228" s="2" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="S228" s="21">
         <v>500000</v>
@@ -38205,13 +38615,13 @@
     </row>
     <row r="229" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A229" s="13" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C229" s="13" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="D229" s="23">
         <v>60</v>
@@ -38253,7 +38663,7 @@
         <v>98</v>
       </c>
       <c r="Q229" s="2" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="R229" t="s">
         <v>146</v>
@@ -38271,7 +38681,7 @@
         <v>0</v>
       </c>
       <c r="W229" s="47" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="X229" s="57">
         <v>0</v>
@@ -38282,13 +38692,13 @@
     </row>
     <row r="230" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A230" s="13" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C230" s="13" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="D230" s="23">
         <v>35</v>
@@ -38333,7 +38743,7 @@
         <v>146</v>
       </c>
       <c r="R230" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="S230" s="20">
         <v>0</v>
@@ -38359,13 +38769,13 @@
     </row>
     <row r="231" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A231" s="13" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="C231" s="13" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D231" s="23">
         <v>37</v>
@@ -38410,7 +38820,7 @@
         <v>146</v>
       </c>
       <c r="R231" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="S231" s="20">
         <v>0</v>
@@ -38436,13 +38846,13 @@
     </row>
     <row r="232" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A232" s="13" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C232" s="13" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="D232" s="23">
         <v>38</v>
@@ -38487,7 +38897,7 @@
         <v>146</v>
       </c>
       <c r="R232" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="S232" s="20">
         <v>0</v>
@@ -38513,13 +38923,13 @@
     </row>
     <row r="233" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A233" s="13" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="C233" s="13" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="D233" s="23">
         <v>39</v>
@@ -38564,7 +38974,7 @@
         <v>146</v>
       </c>
       <c r="R233" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="S233" s="20">
         <v>0</v>
@@ -38590,13 +39000,13 @@
     </row>
     <row r="234" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A234" s="13" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C234" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="D234" s="23">
         <v>44</v>
@@ -38638,10 +39048,10 @@
         <v>0</v>
       </c>
       <c r="Q234" s="2" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="R234" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="S234" s="20">
         <v>0</v>
@@ -38667,13 +39077,13 @@
     </row>
     <row r="235" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A235" s="13" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C235" s="13" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="D235" s="23">
         <v>40</v>
@@ -38744,13 +39154,13 @@
     </row>
     <row r="236" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A236" s="13" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C236" s="13" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="D236" s="23">
         <v>41</v>
@@ -38795,7 +39205,7 @@
         <v>146</v>
       </c>
       <c r="R236" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="S236" s="20">
         <v>0</v>
@@ -38821,13 +39231,13 @@
     </row>
     <row r="237" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A237" s="13" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B237" s="13" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C237" s="13" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D237" s="23">
         <v>42</v>
@@ -38872,7 +39282,7 @@
         <v>146</v>
       </c>
       <c r="R237" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="S237" s="20">
         <v>0</v>
@@ -38898,13 +39308,13 @@
     </row>
     <row r="238" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A238" s="13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="D238" s="23">
         <v>43</v>
@@ -38949,7 +39359,7 @@
         <v>146</v>
       </c>
       <c r="R238" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="S238" s="20">
         <v>0</v>
@@ -38975,13 +39385,13 @@
     </row>
     <row r="239" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A239" s="13" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="C239" s="13" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="D239" s="23">
         <v>44</v>
@@ -39026,7 +39436,7 @@
         <v>146</v>
       </c>
       <c r="R239" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="S239" s="20">
         <v>0</v>
@@ -39052,13 +39462,13 @@
     </row>
     <row r="240" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A240" s="13" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="D240" s="23">
         <v>45</v>
@@ -39103,7 +39513,7 @@
         <v>146</v>
       </c>
       <c r="R240" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="S240" s="20">
         <v>0</v>
@@ -39129,13 +39539,13 @@
     </row>
     <row r="241" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A241" s="13" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D241" s="23">
         <v>45</v>
@@ -39180,7 +39590,7 @@
         <v>146</v>
       </c>
       <c r="R241" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="S241" s="20">
         <v>0</v>
@@ -39206,13 +39616,13 @@
     </row>
     <row r="242" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D242" s="23">
         <v>45</v>
@@ -39257,7 +39667,7 @@
         <v>146</v>
       </c>
       <c r="R242" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="S242" s="20">
         <v>0</v>
@@ -39283,13 +39693,13 @@
     </row>
     <row r="243" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C243" s="13" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="D243" s="23">
         <v>46</v>
@@ -39334,7 +39744,7 @@
         <v>146</v>
       </c>
       <c r="R243" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="S243" s="20">
         <v>0</v>
@@ -39360,13 +39770,13 @@
     </row>
     <row r="244" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C244" s="13" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="D244" s="23">
         <v>72</v>
@@ -39411,7 +39821,7 @@
         <v>146</v>
       </c>
       <c r="R244" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="S244" s="20">
         <v>0</v>
@@ -39426,7 +39836,7 @@
         <v>0</v>
       </c>
       <c r="W244" s="47" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="X244" s="57">
         <v>1</v>
@@ -39437,13 +39847,13 @@
     </row>
     <row r="245" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C245" s="13" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="D245" s="23">
         <v>74</v>
@@ -39514,13 +39924,13 @@
     </row>
     <row r="246" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A246" s="12" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B246" s="12" t="s">
         <v>1313</v>
       </c>
-      <c r="B246" s="12" t="s">
-        <v>1314</v>
-      </c>
       <c r="C246" s="12" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D246" s="23">
         <v>24</v>
@@ -39562,10 +39972,10 @@
         <v>50</v>
       </c>
       <c r="Q246" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="R246" t="s">
-        <v>1316</v>
+        <v>1392</v>
       </c>
       <c r="S246" s="20">
         <v>10</v>
@@ -39587,6 +39997,83 @@
       </c>
       <c r="Y246" s="43">
         <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A247" s="12" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B247" s="12" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C247" s="12" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D247" s="23">
+        <v>22</v>
+      </c>
+      <c r="E247" s="33">
+        <v>2100</v>
+      </c>
+      <c r="F247" s="35">
+        <v>2100</v>
+      </c>
+      <c r="G247" s="41">
+        <v>25</v>
+      </c>
+      <c r="H247" s="25">
+        <v>90</v>
+      </c>
+      <c r="I247" s="24">
+        <v>10</v>
+      </c>
+      <c r="J247" s="34">
+        <v>200</v>
+      </c>
+      <c r="K247" s="26">
+        <v>0</v>
+      </c>
+      <c r="L247" s="27">
+        <v>30</v>
+      </c>
+      <c r="M247" s="17">
+        <v>0</v>
+      </c>
+      <c r="N247" s="3">
+        <v>90</v>
+      </c>
+      <c r="O247" s="29">
+        <v>-100</v>
+      </c>
+      <c r="P247" s="18">
+        <v>25</v>
+      </c>
+      <c r="Q247" s="2" t="s">
+        <v>1391</v>
+      </c>
+      <c r="R247" t="s">
+        <v>1393</v>
+      </c>
+      <c r="S247" s="20">
+        <v>900</v>
+      </c>
+      <c r="T247" s="31">
+        <v>0</v>
+      </c>
+      <c r="U247" s="38">
+        <v>1</v>
+      </c>
+      <c r="V247" s="36">
+        <v>0</v>
+      </c>
+      <c r="W247" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="X247" s="57">
+        <v>0</v>
+      </c>
+      <c r="Y247" s="43">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix inconsistencies and oddities
</commit_message>
<xml_diff>
--- a/data/Data Spreadsheet.xlsx
+++ b/data/Data Spreadsheet.xlsx
@@ -4325,9 +4325,6 @@
     <t>{'Kills': ('Border Guard', 5)}</t>
   </si>
   <si>
-    <t>Kill 5 Border Guards for Bartender Zhang in Pristina.</t>
-  </si>
-  <si>
     <t>Business as Usual</t>
   </si>
   <si>
@@ -4772,15 +4769,6 @@
     <t>A Sword for an Oseku</t>
   </si>
   <si>
-    <t>Bring an Espadon to Qendresa in Pec.</t>
-  </si>
-  <si>
-    <t>Bring a Steel Cuirass to Qendresa in Pec.</t>
-  </si>
-  <si>
-    <t>Find and return the Oseku Shield to Qendresa in Pec.</t>
-  </si>
-  <si>
     <t>Suited in Steel</t>
   </si>
   <si>
@@ -4857,6 +4845,18 @@
   </si>
   <si>
     <t>{'No Criteria': True}</t>
+  </si>
+  <si>
+    <t>Kill 5 Rogue Guards for Bartender Zhang in Pristina.</t>
+  </si>
+  <si>
+    <t>Bring an Espadon to the woman in Pec.</t>
+  </si>
+  <si>
+    <t>Bring a Steel Cuirass to the woman in Pec.</t>
+  </si>
+  <si>
+    <t>Find the lost Oseku Shield somewhere in Albania and return it to the woman in Pec.</t>
   </si>
 </sst>
 </file>
@@ -6044,11 +6044,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127630336"/>
-        <c:axId val="127660800"/>
+        <c:axId val="147122048"/>
+        <c:axId val="147123584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127630336"/>
+        <c:axId val="147122048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6058,7 +6058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127660800"/>
+        <c:crossAx val="147123584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6066,7 +6066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127660800"/>
+        <c:axId val="147123584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000"/>
@@ -6078,7 +6078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127630336"/>
+        <c:crossAx val="147122048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6769,11 +6769,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128038016"/>
-        <c:axId val="128039936"/>
+        <c:axId val="146759680"/>
+        <c:axId val="146761600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128038016"/>
+        <c:axId val="146759680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6801,7 +6801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128039936"/>
+        <c:crossAx val="146761600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6811,7 +6811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128039936"/>
+        <c:axId val="146761600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6822,7 +6822,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128038016"/>
+        <c:crossAx val="146759680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9456,7 +9456,7 @@
         <v>157</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D43" s="64">
         <v>10</v>
@@ -9552,7 +9552,7 @@
         <v>167</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D46" s="64">
         <v>15</v>
@@ -9648,7 +9648,7 @@
         <v>157</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D49" s="64">
         <v>30</v>
@@ -9712,7 +9712,7 @@
         <v>171</v>
       </c>
       <c r="C51" s="64" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D51" s="64">
         <v>50</v>
@@ -13066,7 +13066,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B156" s="12" t="s">
         <v>249</v>
@@ -13090,7 +13090,7 @@
         <v>146</v>
       </c>
       <c r="I156" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="J156" t="s">
         <v>155</v>
@@ -13098,13 +13098,13 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B157" s="12" t="s">
         <v>157</v>
       </c>
       <c r="C157" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -13122,7 +13122,7 @@
         <v>146</v>
       </c>
       <c r="I157" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="J157" t="s">
         <v>155</v>
@@ -17467,7 +17467,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B16" s="43">
         <v>600</v>
@@ -18830,7 +18830,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B63" s="43">
         <v>1225</v>
@@ -18848,7 +18848,7 @@
         <v>125</v>
       </c>
       <c r="G63" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="H63">
         <v>10</v>
@@ -20002,7 +20002,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1600</v>
+        <v>1596</v>
       </c>
       <c r="B57" s="43">
         <v>1225</v>
@@ -21099,13 +21099,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B8" s="43">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>1490</v>
-      </c>
-      <c r="B8" s="43">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>1491</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -21170,7 +21170,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -21297,7 +21297,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G49"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21327,10 +21327,10 @@
         <v>1363</v>
       </c>
       <c r="F1" s="98" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G1" s="98" t="s">
         <v>1558</v>
-      </c>
-      <c r="G1" s="98" t="s">
-        <v>1559</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -21338,7 +21338,7 @@
         <v>1370</v>
       </c>
       <c r="B2" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="C2" t="s">
         <v>1372</v>
@@ -21361,7 +21361,7 @@
         <v>1371</v>
       </c>
       <c r="B3" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="C3" t="s">
         <v>1373</v>
@@ -21381,10 +21381,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="B4" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="C4" t="s">
         <v>1374</v>
@@ -21456,7 +21456,7 @@
         <v>1394</v>
       </c>
       <c r="C7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D7" t="s">
         <v>1397</v>
@@ -21542,10 +21542,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B11" t="s">
-        <v>1432</v>
+        <v>1606</v>
       </c>
       <c r="C11" t="s">
         <v>1431</v>
@@ -21565,13 +21565,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B12" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C12" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D12" t="s">
         <v>1427</v>
@@ -21588,13 +21588,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B13" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C13" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D13" t="s">
         <v>1429</v>
@@ -21611,19 +21611,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B14" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="C14" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D14" t="s">
         <v>1369</v>
       </c>
       <c r="E14" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="F14" s="98">
         <v>0</v>
@@ -21640,7 +21640,7 @@
         <v>1404</v>
       </c>
       <c r="C15" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D15" t="s">
         <v>411</v>
@@ -21657,19 +21657,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B16" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="C16" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="D16" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E16" t="s">
         <v>1462</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1463</v>
       </c>
       <c r="F16" s="98">
         <v>0</v>
@@ -21680,19 +21680,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B17" t="s">
         <v>1465</v>
       </c>
-      <c r="B17" t="s">
-        <v>1466</v>
-      </c>
       <c r="C17" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D17" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="E17" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="F17" s="98">
         <v>0</v>
@@ -21703,19 +21703,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B18" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E18" t="s">
         <v>1469</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1609</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1468</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1470</v>
       </c>
       <c r="F18" s="98">
         <v>0</v>
@@ -21732,7 +21732,7 @@
         <v>1409</v>
       </c>
       <c r="C19" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D19" t="s">
         <v>1406</v>
@@ -21749,19 +21749,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B20" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="C20" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D20" t="s">
         <v>1407</v>
       </c>
       <c r="E20" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="F20" s="98">
         <v>0</v>
@@ -21772,19 +21772,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B21" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C21" t="s">
         <v>1452</v>
       </c>
-      <c r="C21" t="s">
-        <v>1453</v>
-      </c>
       <c r="D21" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="E21" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="F21" s="98">
         <v>0</v>
@@ -21795,19 +21795,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B22" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="C22" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D22" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="E22" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="F22" s="98">
         <v>0</v>
@@ -21818,19 +21818,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E23" t="s">
         <v>1457</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1460</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1609</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1459</v>
-      </c>
-      <c r="E23" t="s">
-        <v>1458</v>
       </c>
       <c r="F23" s="98">
         <v>0</v>
@@ -21841,19 +21841,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B24" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1472</v>
+      </c>
+      <c r="E24" t="s">
         <v>1475</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1474</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1473</v>
-      </c>
-      <c r="E24" t="s">
-        <v>1476</v>
       </c>
       <c r="F24" s="98">
         <v>0</v>
@@ -21864,19 +21864,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B25" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="C25" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="D25" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="E25" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="F25" s="98">
         <v>0</v>
@@ -21887,19 +21887,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D26" t="s">
         <v>1483</v>
       </c>
-      <c r="B26" t="s">
-        <v>1485</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1609</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1484</v>
-      </c>
       <c r="E26" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="F26" s="98">
         <v>0</v>
@@ -21910,19 +21910,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B27" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C27" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D27" t="s">
         <v>1486</v>
       </c>
-      <c r="D27" t="s">
-        <v>1487</v>
-      </c>
       <c r="E27" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="F27" s="98">
         <v>0</v>
@@ -21933,19 +21933,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C28" t="s">
         <v>1499</v>
       </c>
-      <c r="B28" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1500</v>
-      </c>
       <c r="D28" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="E28" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="F28" s="98">
         <v>0</v>
@@ -21956,19 +21956,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="B29" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C29" t="s">
         <v>1495</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E29" t="s">
         <v>1496</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1493</v>
-      </c>
-      <c r="E29" t="s">
-        <v>1497</v>
       </c>
       <c r="F29" s="98">
         <v>0</v>
@@ -21979,19 +21979,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="B30" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="C30" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="D30" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E30" t="s">
         <v>1503</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1504</v>
       </c>
       <c r="F30" s="98">
         <v>0</v>
@@ -22002,19 +22002,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B31" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C31" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D31" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="E31" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="F31" s="98">
         <v>0</v>
@@ -22025,19 +22025,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="B32" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C32" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D32" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="E32" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="F32" s="98">
         <v>0</v>
@@ -22048,19 +22048,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B33" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="C33" t="s">
         <v>1382</v>
       </c>
       <c r="D33" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="E33" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="F33" s="98">
         <v>0</v>
@@ -22077,10 +22077,10 @@
         <v>1381</v>
       </c>
       <c r="C34" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="D34" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="E34" t="s">
         <v>1380</v>
@@ -22094,19 +22094,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B35" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="C35" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D35" t="s">
         <v>1380</v>
       </c>
       <c r="E35" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="F35" s="98">
         <v>0</v>
@@ -22117,19 +22117,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B36" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="C36" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="D36" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="E36" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="F36" s="98">
         <v>0</v>
@@ -22140,19 +22140,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B37" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C37" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D37" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E37" t="s">
         <v>1535</v>
-      </c>
-      <c r="E37" t="s">
-        <v>1536</v>
       </c>
       <c r="F37" s="98">
         <v>0</v>
@@ -22163,19 +22163,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1597</v>
+      </c>
+      <c r="D38" t="s">
         <v>1540</v>
       </c>
-      <c r="B38" t="s">
-        <v>1543</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1601</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>1541</v>
-      </c>
-      <c r="E38" t="s">
-        <v>1542</v>
       </c>
       <c r="F38" s="98">
         <v>0</v>
@@ -22186,19 +22186,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1601</v>
+      </c>
+      <c r="D39" t="s">
         <v>1544</v>
       </c>
-      <c r="B39" t="s">
-        <v>1550</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1605</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>1545</v>
-      </c>
-      <c r="E39" t="s">
-        <v>1546</v>
       </c>
       <c r="F39" s="98">
         <v>0</v>
@@ -22209,19 +22209,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="B40" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C40" t="s">
-        <v>1604</v>
+        <v>1600</v>
       </c>
       <c r="D40" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="E40" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F40" s="98">
         <v>0</v>
@@ -22255,19 +22255,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B42" t="s">
-        <v>1608</v>
+        <v>1604</v>
       </c>
       <c r="C42" t="s">
-        <v>1602</v>
+        <v>1598</v>
       </c>
       <c r="D42" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="E42" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F42" s="98">
         <v>1</v>
@@ -22278,19 +22278,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1602</v>
+      </c>
+      <c r="D43" t="s">
         <v>1552</v>
       </c>
-      <c r="B43" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1606</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>1553</v>
-      </c>
-      <c r="E43" t="s">
-        <v>1554</v>
       </c>
       <c r="F43" s="98">
         <v>1</v>
@@ -22301,19 +22301,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="B44" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1561</v>
+      </c>
+      <c r="E44" t="s">
         <v>1560</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1563</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1562</v>
-      </c>
-      <c r="E44" t="s">
-        <v>1561</v>
       </c>
       <c r="F44" s="98">
         <v>1</v>
@@ -22324,19 +22324,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>1586</v>
+        <v>1582</v>
       </c>
       <c r="B45" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C45" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D45" t="s">
         <v>1565</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>1566</v>
-      </c>
-      <c r="E45" t="s">
-        <v>1567</v>
       </c>
       <c r="F45" s="98">
         <v>1</v>
@@ -22347,19 +22347,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
       <c r="B46" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C46" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="D46" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="E46" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="F46" s="98">
         <v>1</v>
@@ -22370,19 +22370,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="B47" t="s">
-        <v>1581</v>
+        <v>1607</v>
       </c>
       <c r="C47" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="D47" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E47" t="s">
         <v>1572</v>
-      </c>
-      <c r="E47" t="s">
-        <v>1573</v>
       </c>
       <c r="F47" s="98">
         <v>0</v>
@@ -22393,19 +22393,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="B48" t="s">
-        <v>1582</v>
+        <v>1608</v>
       </c>
       <c r="C48" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D48" t="s">
+        <v>1572</v>
+      </c>
+      <c r="E48" t="s">
         <v>1573</v>
-      </c>
-      <c r="E48" t="s">
-        <v>1574</v>
       </c>
       <c r="F48" s="98">
         <v>0</v>
@@ -22416,19 +22416,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B49" t="s">
-        <v>1583</v>
+        <v>1609</v>
       </c>
       <c r="C49" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="D49" t="s">
+        <v>1573</v>
+      </c>
+      <c r="E49" t="s">
         <v>1574</v>
-      </c>
-      <c r="E49" t="s">
-        <v>1575</v>
       </c>
       <c r="F49" s="98">
         <v>0</v>
@@ -22439,19 +22439,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B50" t="s">
         <v>1588</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D50" t="s">
         <v>1592</v>
       </c>
-      <c r="C50" t="s">
-        <v>1609</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1596</v>
-      </c>
       <c r="E50" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="F50" s="98">
         <v>0</v>
@@ -22462,19 +22462,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
       <c r="B51" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D51" t="s">
         <v>1593</v>
       </c>
-      <c r="C51" t="s">
-        <v>1609</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1597</v>
-      </c>
       <c r="E51" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="F51" s="98">
         <v>0</v>
@@ -22485,19 +22485,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="B52" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D52" t="s">
         <v>1594</v>
       </c>
-      <c r="C52" t="s">
-        <v>1609</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1598</v>
-      </c>
       <c r="E52" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="F52" s="98">
         <v>0</v>
@@ -22519,10 +22519,10 @@
   <dimension ref="A1:Y248"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E193" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A248" sqref="A248"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -41576,13 +41576,13 @@
     </row>
     <row r="248" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A248" s="12" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C248" s="12" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D248" s="23">
         <v>6</v>
@@ -41624,10 +41624,10 @@
         <v>-100</v>
       </c>
       <c r="Q248" s="2" t="s">
+        <v>1509</v>
+      </c>
+      <c r="R248" s="2" t="s">
         <v>1510</v>
-      </c>
-      <c r="R248" s="2" t="s">
-        <v>1511</v>
       </c>
       <c r="S248" s="21">
         <v>100</v>

</xml_diff>

<commit_message>
Improve special battle actions
- Allow potion use in battle
- Synchronize equipping items in battle with turn order
</commit_message>
<xml_diff>
--- a/data/Data Spreadsheet.xlsx
+++ b/data/Data Spreadsheet.xlsx
@@ -6056,11 +6056,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127106048"/>
-        <c:axId val="129311488"/>
+        <c:axId val="108104704"/>
+        <c:axId val="124850944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127106048"/>
+        <c:axId val="108104704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6070,7 +6070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129311488"/>
+        <c:crossAx val="124850944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6078,7 +6078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129311488"/>
+        <c:axId val="124850944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000"/>
@@ -6090,7 +6090,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127106048"/>
+        <c:crossAx val="108104704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6781,11 +6781,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="125797504"/>
-        <c:axId val="125799424"/>
+        <c:axId val="125195392"/>
+        <c:axId val="125197312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125797504"/>
+        <c:axId val="125195392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6813,7 +6813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125799424"/>
+        <c:crossAx val="125197312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6823,7 +6823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125799424"/>
+        <c:axId val="125197312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6834,7 +6834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125797504"/>
+        <c:crossAx val="125195392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8105,7 +8105,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="A1:J158"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10843,7 +10843,7 @@
         <v>1612</v>
       </c>
       <c r="B86" s="96" t="s">
-        <v>636</v>
+        <v>249</v>
       </c>
       <c r="C86" s="96" t="s">
         <v>159</v>
@@ -10852,7 +10852,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="97">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F86" s="96" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Add event item and change how events are displayed
</commit_message>
<xml_diff>
--- a/data/Data Spreadsheet.xlsx
+++ b/data/Data Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="7"/>
+    <workbookView xWindow="9750" yWindow="345" windowWidth="15810" windowHeight="12825" tabRatio="621" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EXP" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="1390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3414" uniqueCount="1391">
   <si>
     <t>Club</t>
   </si>
@@ -4197,6 +4197,9 @@
   </si>
   <si>
     <t>{'Items': {'Key Mold': 1}}</t>
+  </si>
+  <si>
+    <t>Hopalong Boots</t>
   </si>
 </sst>
 </file>
@@ -5383,11 +5386,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="124673024"/>
-        <c:axId val="124707584"/>
+        <c:axId val="127036416"/>
+        <c:axId val="127992576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124673024"/>
+        <c:axId val="127036416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5397,7 +5400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124707584"/>
+        <c:crossAx val="127992576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5405,7 +5408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124707584"/>
+        <c:axId val="127992576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000"/>
@@ -5417,7 +5420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124673024"/>
+        <c:crossAx val="127036416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6108,11 +6111,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126465152"/>
-        <c:axId val="126467072"/>
+        <c:axId val="128038016"/>
+        <c:axId val="128039936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126465152"/>
+        <c:axId val="128038016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6140,7 +6143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126467072"/>
+        <c:crossAx val="128039936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6150,7 +6153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126467072"/>
+        <c:axId val="128039936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6161,7 +6164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126465152"/>
+        <c:crossAx val="128038016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18086,11 +18089,9 @@
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:F55"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19195,6 +19196,26 @@
       </c>
       <c r="F55">
         <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B56" s="43">
+        <v>1225</v>
+      </c>
+      <c r="C56" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" s="27">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -20461,7 +20482,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>

</xml_diff>